<commit_message>
Increase to 10 executions
</commit_message>
<xml_diff>
--- a/outputs/paper/ARR_Rank.xlsx
+++ b/outputs/paper/ARR_Rank.xlsx
@@ -88,40 +88,40 @@
     <t>BottomUp Rank</t>
   </si>
   <si>
+    <t>BottomUp L1</t>
+  </si>
+  <si>
+    <t>Window AR</t>
+  </si>
+  <si>
+    <t>BottomUp RBF</t>
+  </si>
+  <si>
     <t>BottomUp AR</t>
   </si>
   <si>
-    <t>BottomUp L1</t>
-  </si>
-  <si>
-    <t>Window AR</t>
-  </si>
-  <si>
-    <t>BottomUp RBF</t>
-  </si>
-  <si>
     <t>Window L2</t>
   </si>
   <si>
     <t>BinSeg Normal</t>
   </si>
   <si>
+    <t>BottomUp L2</t>
+  </si>
+  <si>
     <t>BottomUp Normal</t>
   </si>
   <si>
-    <t>BottomUp L2</t>
+    <t>BinSeg Rank</t>
+  </si>
+  <si>
+    <t>Window Normal</t>
   </si>
   <si>
     <t>BinSeg L1</t>
   </si>
   <si>
-    <t>Window Normal</t>
-  </si>
-  <si>
-    <t>BinSeg Rank</t>
-  </si>
-  <si>
-    <t>Full</t>
+    <t>No CPD</t>
   </si>
   <si>
     <t>BinSeg RBF</t>
@@ -139,10 +139,10 @@
     <t>BinSeg L2</t>
   </si>
   <si>
+    <t>Window Linear</t>
+  </si>
+  <si>
     <t>BinSeg AR</t>
-  </si>
-  <si>
-    <t>Window Linear</t>
   </si>
 </sst>
 </file>
@@ -576,61 +576,61 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>1.098446139545976</v>
+        <v>1.096475584272148</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1.110892828764933</v>
+        <v>1.108945552742671</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>1.131360941814583</v>
+        <v>1.129324259537674</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
       <c r="H2">
-        <v>1.162653503539676</v>
+        <v>1.160815804357349</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2">
-        <v>1.217101467165406</v>
+        <v>1.220392935599892</v>
       </c>
       <c r="K2">
         <v>5</v>
       </c>
       <c r="L2">
-        <v>1.215298371460702</v>
+        <v>1.207007661777844</v>
       </c>
       <c r="M2">
         <v>10</v>
       </c>
       <c r="N2">
-        <v>1.278569174012918</v>
+        <v>1.265981068401369</v>
       </c>
       <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <v>1.364987252664707</v>
+      </c>
+      <c r="Q2">
         <v>9</v>
       </c>
-      <c r="P2">
-        <v>1.38720385446601</v>
-      </c>
-      <c r="Q2">
-        <v>8</v>
-      </c>
       <c r="R2">
-        <v>1.449823247179991</v>
+        <v>1.375559274084418</v>
       </c>
       <c r="S2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="T2">
-        <v>1.667635576542297</v>
+        <v>1.66287794110657</v>
       </c>
       <c r="U2">
         <v>4</v>
@@ -641,61 +641,61 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>1.097961101085476</v>
+        <v>1.083044553220067</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1.121665441885213</v>
+        <v>1.107323626900181</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>1.154175981593707</v>
+        <v>1.140468958653252</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3">
-        <v>1.199155288117408</v>
+        <v>1.186884643582913</v>
       </c>
       <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>1.272641677055092</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>1.266604950497278</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>1.353977844572786</v>
+      </c>
+      <c r="O3">
+        <v>9</v>
+      </c>
+      <c r="P3">
+        <v>1.512181813345827</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <v>1.559643008779139</v>
+      </c>
+      <c r="S3">
         <v>4</v>
       </c>
-      <c r="J3">
-        <v>1.272284383962108</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>1.282581856013343</v>
-      </c>
-      <c r="M3">
-        <v>7</v>
-      </c>
-      <c r="N3">
-        <v>1.37023301034011</v>
-      </c>
-      <c r="O3">
-        <v>8</v>
-      </c>
-      <c r="P3">
-        <v>1.524125153617817</v>
-      </c>
-      <c r="Q3">
-        <v>6</v>
-      </c>
-      <c r="R3">
-        <v>1.638212344521357</v>
-      </c>
-      <c r="S3">
-        <v>3</v>
-      </c>
       <c r="T3">
-        <v>1.805265980771527</v>
+        <v>1.795496870031311</v>
       </c>
       <c r="U3">
         <v>3</v>
@@ -706,61 +706,61 @@
         <v>23</v>
       </c>
       <c r="B4">
-        <v>1.077261585139405</v>
+        <v>1.061734415868065</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
-        <v>1.05287544393936</v>
+        <v>1.037835804742023</v>
       </c>
       <c r="E4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>1.033203290692545</v>
+        <v>1.018552709137146</v>
       </c>
       <c r="G4">
         <v>14</v>
       </c>
       <c r="H4">
-        <v>1.017446481484358</v>
+        <v>1.003177443884919</v>
       </c>
       <c r="I4">
         <v>16</v>
       </c>
       <c r="J4">
-        <v>1.005250887569882</v>
+        <v>0.991459677920928</v>
       </c>
       <c r="K4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L4">
-        <v>0.9966377533572419</v>
+        <v>0.9835929892260958</v>
       </c>
       <c r="M4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N4">
-        <v>0.9921523102456555</v>
+        <v>0.9805246370373211</v>
       </c>
       <c r="O4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P4">
-        <v>0.9935779588313074</v>
+        <v>0.9854805607832389</v>
       </c>
       <c r="Q4">
         <v>15</v>
       </c>
       <c r="R4">
-        <v>1.008324543629652</v>
+        <v>1.0206703454613</v>
       </c>
       <c r="S4">
         <v>15</v>
       </c>
       <c r="T4">
-        <v>0.9454073043900297</v>
+        <v>0.9323900882262983</v>
       </c>
       <c r="U4">
         <v>19</v>
@@ -771,64 +771,64 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>1.067024606252472</v>
+        <v>1.06168206144241</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>1.062093106035909</v>
+        <v>1.037550890315733</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F5">
-        <v>1.062280618961817</v>
+        <v>1.018067408332517</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H5">
-        <v>1.067925528783702</v>
+        <v>1.002447521994901</v>
       </c>
       <c r="I5">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J5">
-        <v>1.080856002051197</v>
+        <v>0.9903102060396979</v>
       </c>
       <c r="K5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L5">
-        <v>1.109218952749107</v>
+        <v>0.9815798483004586</v>
       </c>
       <c r="M5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="N5">
-        <v>1.075581066320229</v>
+        <v>0.9765125137726514</v>
       </c>
       <c r="O5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="P5">
-        <v>1.09400380836192</v>
+        <v>0.975878102713619</v>
       </c>
       <c r="Q5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="R5">
-        <v>1.12116840332787</v>
+        <v>0.9815467970555257</v>
       </c>
       <c r="S5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="T5">
-        <v>1.162331533524324</v>
+        <v>0.9988408130274806</v>
       </c>
       <c r="U5">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -836,64 +836,64 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>1.061127048814572</v>
+        <v>1.058952224396026</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>1.033908921979554</v>
+        <v>1.065463092552758</v>
       </c>
       <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>1.077625891559313</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>1.096365094036048</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>1.125004877764473</v>
+      </c>
+      <c r="K6">
         <v>11</v>
       </c>
-      <c r="F6">
-        <v>1.011539631994509</v>
-      </c>
-      <c r="G6">
-        <v>16</v>
-      </c>
-      <c r="H6">
-        <v>0.9930866118420686</v>
-      </c>
-      <c r="I6">
-        <v>18</v>
-      </c>
-      <c r="J6">
-        <v>0.9780206596883303</v>
-      </c>
-      <c r="K6">
-        <v>17</v>
-      </c>
       <c r="L6">
-        <v>0.9660775714815875</v>
+        <v>1.183237853029777</v>
       </c>
       <c r="M6">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="N6">
-        <v>0.9572193029574226</v>
+        <v>1.150480176543564</v>
       </c>
       <c r="O6">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="P6">
-        <v>0.951666138062446</v>
+        <v>1.199207167687442</v>
       </c>
       <c r="Q6">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="R6">
-        <v>0.950031849678332</v>
+        <v>1.335253020657419</v>
       </c>
       <c r="S6">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="T6">
-        <v>0.9537134537419147</v>
+        <v>1.182581769876504</v>
       </c>
       <c r="U6">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -901,64 +901,64 @@
         <v>26</v>
       </c>
       <c r="B7">
-        <v>1.058851674230974</v>
+        <v>1.056713680158891</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7">
-        <v>1.064044398892955</v>
+        <v>1.034554507371336</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>1.074792469006759</v>
+        <v>1.016927619901871</v>
       </c>
       <c r="G7">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H7">
-        <v>1.091707898922447</v>
+        <v>1.003108048869777</v>
       </c>
       <c r="I7">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J7">
-        <v>1.117136022204702</v>
+        <v>0.9927639577272055</v>
       </c>
       <c r="K7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L7">
-        <v>1.161203862302077</v>
+        <v>0.985869993492374</v>
       </c>
       <c r="M7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N7">
-        <v>1.142493599425352</v>
+        <v>0.9827444962927927</v>
       </c>
       <c r="O7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="P7">
-        <v>1.183495744064609</v>
+        <v>0.9842495027125165</v>
       </c>
       <c r="Q7">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R7">
-        <v>1.249455388764074</v>
+        <v>0.9924175904561233</v>
       </c>
       <c r="S7">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="T7">
-        <v>1.184628329184237</v>
+        <v>1.012931142430802</v>
       </c>
       <c r="U7">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -966,64 +966,64 @@
         <v>27</v>
       </c>
       <c r="B8">
-        <v>1.054270819750176</v>
+        <v>1.054116764341472</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>1.03155017235567</v>
+        <v>1.049404659884196</v>
       </c>
       <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>1.049724245589476</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>1.05558859434869</v>
+      </c>
+      <c r="I8">
         <v>13</v>
       </c>
-      <c r="F8">
-        <v>1.013433246892508</v>
-      </c>
-      <c r="G8">
-        <v>15</v>
-      </c>
-      <c r="H8">
-        <v>0.9991140540915096</v>
-      </c>
-      <c r="I8">
-        <v>17</v>
-      </c>
       <c r="J8">
-        <v>0.9881706909539749</v>
+        <v>1.069426244902838</v>
       </c>
       <c r="K8">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L8">
-        <v>0.9804496535544166</v>
+        <v>1.105152946524391</v>
       </c>
       <c r="M8">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N8">
-        <v>0.9760501389635465</v>
+        <v>1.059667314329371</v>
       </c>
       <c r="O8">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P8">
-        <v>0.9753936255838919</v>
+        <v>1.077039746571793</v>
       </c>
       <c r="Q8">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="R8">
-        <v>0.9794394848427408</v>
+        <v>1.103058796180808</v>
       </c>
       <c r="S8">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="T8">
-        <v>0.9902917949847799</v>
+        <v>1.143367150280038</v>
       </c>
       <c r="U8">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1031,64 +1031,64 @@
         <v>28</v>
       </c>
       <c r="B9">
-        <v>1.049645010465107</v>
+        <v>1.050726750301721</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9">
-        <v>1.069278324536235</v>
+        <v>1.070241863579622</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
       <c r="F9">
-        <v>1.095474028557689</v>
+        <v>1.096334869188334</v>
       </c>
       <c r="G9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>1.129767629255009</v>
+        <v>1.130784761306789</v>
       </c>
       <c r="I9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J9">
-        <v>1.176238936677345</v>
+        <v>1.178609731005983</v>
       </c>
       <c r="K9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L9">
-        <v>1.252903927335987</v>
+        <v>1.270138820504554</v>
       </c>
       <c r="M9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N9">
-        <v>1.244205289134586</v>
+        <v>1.24367355569919</v>
       </c>
       <c r="O9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P9">
-        <v>1.327196317343978</v>
+        <v>1.346383320853301</v>
       </c>
       <c r="Q9">
         <v>11</v>
       </c>
       <c r="R9">
-        <v>1.292040104495872</v>
+        <v>1.273831233825431</v>
       </c>
       <c r="S9">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="T9">
-        <v>1.489520488614116</v>
+        <v>1.409481862005331</v>
       </c>
       <c r="U9">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1096,64 +1096,64 @@
         <v>29</v>
       </c>
       <c r="B10">
-        <v>1.041631208085537</v>
+        <v>1.048957970551326</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10">
-        <v>1.066598639132925</v>
+        <v>1.075237682281905</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>1.101313624806495</v>
+        <v>1.111411994790438</v>
       </c>
       <c r="G10">
         <v>6</v>
       </c>
       <c r="H10">
-        <v>1.150520984252484</v>
+        <v>1.162695164216764</v>
       </c>
       <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>1.245891759042389</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>1.264148389521569</v>
+      </c>
+      <c r="M10">
+        <v>7</v>
+      </c>
+      <c r="N10">
+        <v>1.430020511418638</v>
+      </c>
+      <c r="O10">
         <v>6</v>
       </c>
-      <c r="J10">
-        <v>1.228212639408539</v>
-      </c>
-      <c r="K10">
-        <v>4</v>
-      </c>
-      <c r="L10">
-        <v>1.255292756650288</v>
-      </c>
-      <c r="M10">
+      <c r="P10">
+        <v>1.680539705797795</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <v>1.261204666133432</v>
+      </c>
+      <c r="S10">
+        <v>12</v>
+      </c>
+      <c r="T10">
+        <v>1.358376595201438</v>
+      </c>
+      <c r="U10">
         <v>8</v>
-      </c>
-      <c r="N10">
-        <v>1.43829199174358</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="P10">
-        <v>1.667210543336778</v>
-      </c>
-      <c r="Q10">
-        <v>5</v>
-      </c>
-      <c r="R10">
-        <v>1.291046389164475</v>
-      </c>
-      <c r="S10">
-        <v>9</v>
-      </c>
-      <c r="T10">
-        <v>1.223454779515637</v>
-      </c>
-      <c r="U10">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1161,64 +1161,64 @@
         <v>30</v>
       </c>
       <c r="B11">
-        <v>1.037745247578482</v>
+        <v>1.047267780464769</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>1.077577780237288</v>
+        <v>1.069473909618415</v>
       </c>
       <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>1.100216769371</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>1.143319471052173</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <v>1.209856898043752</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>1.394088693868389</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>1.375323296151508</v>
+      </c>
+      <c r="O11">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <v>1.468298542163537</v>
+      </c>
+      <c r="Q11">
+        <v>8</v>
+      </c>
+      <c r="R11">
+        <v>1.68355630308076</v>
+      </c>
+      <c r="S11">
         <v>3</v>
       </c>
-      <c r="F11">
-        <v>1.130725071960521</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>1.205959486007921</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-      <c r="J11">
-        <v>1.338147991801857</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1.402543594462469</v>
-      </c>
-      <c r="M11">
-        <v>4</v>
-      </c>
-      <c r="N11">
-        <v>1.872520452203286</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <v>1.354694060406312</v>
-      </c>
-      <c r="Q11">
-        <v>10</v>
-      </c>
-      <c r="R11">
-        <v>1.409647132741932</v>
-      </c>
-      <c r="S11">
-        <v>7</v>
-      </c>
       <c r="T11">
-        <v>1.427285410021901</v>
+        <v>1.237751447238716</v>
       </c>
       <c r="U11">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1226,64 +1226,64 @@
         <v>31</v>
       </c>
       <c r="B12">
-        <v>1.033535936146831</v>
+        <v>1.031457901664917</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12">
-        <v>1.056739865070445</v>
+        <v>1.067224637040966</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>1.088794530019856</v>
+        <v>1.115029292175002</v>
       </c>
       <c r="G12">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H12">
-        <v>1.133539702032215</v>
+        <v>1.182629051574606</v>
       </c>
       <c r="I12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J12">
-        <v>1.201544668344188</v>
+        <v>1.300514992012559</v>
       </c>
       <c r="K12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>1.366882951277943</v>
+        <v>1.529602474709112</v>
       </c>
       <c r="M12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>1.393559597014552</v>
+        <v>1.581367019433214</v>
       </c>
       <c r="O12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="P12">
-        <v>1.51819724286595</v>
+        <v>1.490724495672699</v>
       </c>
       <c r="Q12">
         <v>7</v>
       </c>
       <c r="R12">
-        <v>1.654152129734367</v>
+        <v>1.548093417153733</v>
       </c>
       <c r="S12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T12">
-        <v>1.225163841173187</v>
+        <v>1.292809807928736</v>
       </c>
       <c r="U12">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1291,64 +1291,64 @@
         <v>32</v>
       </c>
       <c r="B13">
-        <v>1.017693436553732</v>
+        <v>1.02803013132057</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13">
-        <v>0.9953024174829171</v>
+        <v>1.004406533409582</v>
       </c>
       <c r="E13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13">
-        <v>0.9775920819135725</v>
+        <v>0.9853487253403637</v>
       </c>
       <c r="G13">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H13">
-        <v>0.9637392167271889</v>
+        <v>0.9700741443075002</v>
       </c>
       <c r="I13">
         <v>19</v>
       </c>
       <c r="J13">
-        <v>0.9533161235769199</v>
+        <v>0.958192738465202</v>
       </c>
       <c r="K13">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L13">
-        <v>0.9461723873980555</v>
+        <v>0.9496066281806315</v>
       </c>
       <c r="M13">
         <v>19</v>
       </c>
       <c r="N13">
-        <v>0.9424218597124882</v>
+        <v>0.9445245112836312</v>
       </c>
       <c r="O13">
         <v>19</v>
       </c>
       <c r="P13">
-        <v>0.9425226671586535</v>
+        <v>0.9436067279322886</v>
       </c>
       <c r="Q13">
         <v>19</v>
       </c>
       <c r="R13">
-        <v>0.947523434902715</v>
+        <v>0.9484096399780769</v>
       </c>
       <c r="S13">
         <v>19</v>
       </c>
       <c r="T13">
-        <v>0.9597667988620774</v>
+        <v>0.9628940909179671</v>
       </c>
       <c r="U13">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1356,64 +1356,64 @@
         <v>33</v>
       </c>
       <c r="B14">
-        <v>1.015544273422004</v>
+        <v>1.025397174108525</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14">
-        <v>1.032669066016462</v>
+        <v>1.043941349256491</v>
       </c>
       <c r="E14">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>1.056651646744822</v>
+        <v>1.069478536171666</v>
       </c>
       <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>1.104251319208093</v>
+      </c>
+      <c r="I14">
         <v>11</v>
       </c>
-      <c r="H14">
-        <v>1.089437043616437</v>
-      </c>
-      <c r="I14">
-        <v>12</v>
-      </c>
       <c r="J14">
-        <v>1.135641133851651</v>
+        <v>1.153821434507214</v>
       </c>
       <c r="K14">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L14">
-        <v>1.210130669107495</v>
+        <v>1.238993940173276</v>
       </c>
       <c r="M14">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="N14">
-        <v>1.205353566530211</v>
+        <v>1.479604300668834</v>
       </c>
       <c r="O14">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="P14">
-        <v>1.356976005864798</v>
+        <v>1.364321213831999</v>
       </c>
       <c r="Q14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R14">
-        <v>1.459741250336165</v>
+        <v>1.497051654402041</v>
       </c>
       <c r="S14">
+        <v>7</v>
+      </c>
+      <c r="T14">
+        <v>1.539732463524918</v>
+      </c>
+      <c r="U14">
         <v>5</v>
-      </c>
-      <c r="T14">
-        <v>1.851935028021195</v>
-      </c>
-      <c r="U14">
-        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1421,64 +1421,64 @@
         <v>34</v>
       </c>
       <c r="B15">
-        <v>1.012730674383721</v>
+        <v>1.020342092729119</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15">
-        <v>0.9888154456785789</v>
+        <v>0.9983176340959177</v>
       </c>
       <c r="E15">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>0.9808941152373433</v>
+      </c>
+      <c r="G15">
         <v>18</v>
       </c>
-      <c r="F15">
-        <v>0.9694277054880496</v>
-      </c>
-      <c r="G15">
-        <v>19</v>
-      </c>
       <c r="H15">
-        <v>0.9537252086408385</v>
+        <v>0.9673176043190614</v>
       </c>
       <c r="I15">
         <v>20</v>
       </c>
       <c r="J15">
-        <v>0.9412427828232216</v>
+        <v>0.9572339481996606</v>
       </c>
       <c r="K15">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L15">
-        <v>0.9317694781902303</v>
+        <v>0.9505937258283339</v>
       </c>
       <c r="M15">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N15">
-        <v>0.9253198305419916</v>
+        <v>0.9476782309786268</v>
       </c>
       <c r="O15">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P15">
-        <v>0.922176721304277</v>
+        <v>0.9492689631842507</v>
       </c>
       <c r="Q15">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R15">
-        <v>0.9230429920255518</v>
+        <v>0.9571481565715342</v>
       </c>
       <c r="S15">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="T15">
-        <v>0.9294584109187689</v>
+        <v>0.975744149709886</v>
       </c>
       <c r="U15">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1486,61 +1486,61 @@
         <v>35</v>
       </c>
       <c r="B16">
-        <v>1.010160079478638</v>
+        <v>1.008154569172945</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16">
-        <v>0.9520309965080924</v>
+        <v>0.9485495844941579</v>
       </c>
       <c r="E16">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F16">
-        <v>0.9024301691480888</v>
+        <v>0.8977653274531157</v>
       </c>
       <c r="G16">
         <v>22</v>
       </c>
       <c r="H16">
-        <v>0.859452699129116</v>
+        <v>0.853849693151205</v>
       </c>
       <c r="I16">
         <v>22</v>
       </c>
       <c r="J16">
-        <v>0.8218169078623422</v>
+        <v>0.8154890626851603</v>
       </c>
       <c r="K16">
         <v>22</v>
       </c>
       <c r="L16">
-        <v>0.7886193335223995</v>
+        <v>0.7817637863505321</v>
       </c>
       <c r="M16">
         <v>22</v>
       </c>
       <c r="N16">
-        <v>0.7592109012286071</v>
+        <v>0.7520267449376651</v>
       </c>
       <c r="O16">
         <v>22</v>
       </c>
       <c r="P16">
-        <v>0.7331317580472521</v>
+        <v>0.7258457981421534</v>
       </c>
       <c r="Q16">
         <v>22</v>
       </c>
       <c r="R16">
-        <v>0.7100825808604758</v>
+        <v>0.7029950149234478</v>
       </c>
       <c r="S16">
         <v>22</v>
       </c>
       <c r="T16">
-        <v>0.6899297766668384</v>
+        <v>0.6835138664776848</v>
       </c>
       <c r="U16">
         <v>22</v>
@@ -1551,61 +1551,61 @@
         <v>36</v>
       </c>
       <c r="B17">
-        <v>1.006124101527399</v>
+        <v>0.9991030613116985</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17">
-        <v>0.9529701541370263</v>
+        <v>0.9443835163561156</v>
       </c>
       <c r="E17">
         <v>20</v>
       </c>
       <c r="F17">
-        <v>0.9086268574677618</v>
+        <v>0.8988049366539033</v>
       </c>
       <c r="G17">
         <v>21</v>
       </c>
       <c r="H17">
-        <v>0.8708998232265236</v>
+        <v>0.8600908741308049</v>
       </c>
       <c r="I17">
         <v>21</v>
       </c>
       <c r="J17">
-        <v>0.8383858935052561</v>
+        <v>0.8267890765996453</v>
       </c>
       <c r="K17">
         <v>21</v>
       </c>
       <c r="L17">
-        <v>0.8101443609238498</v>
+        <v>0.7979339627052328</v>
       </c>
       <c r="M17">
         <v>21</v>
       </c>
       <c r="N17">
-        <v>0.7855400727286572</v>
+        <v>0.7728888306607634</v>
       </c>
       <c r="O17">
         <v>21</v>
       </c>
       <c r="P17">
-        <v>0.7641701785690665</v>
+        <v>0.7512814850583902</v>
       </c>
       <c r="Q17">
         <v>21</v>
       </c>
       <c r="R17">
-        <v>0.7458497731197765</v>
+        <v>0.7330205308753661</v>
       </c>
       <c r="S17">
         <v>21</v>
       </c>
       <c r="T17">
-        <v>0.7306740233703274</v>
+        <v>0.7184594622480753</v>
       </c>
       <c r="U17">
         <v>21</v>
@@ -1616,64 +1616,64 @@
         <v>37</v>
       </c>
       <c r="B18">
-        <v>0.9655590290159518</v>
+        <v>0.9881495817969133</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18">
-        <v>0.9964312771184022</v>
+        <v>1.019202571983889</v>
       </c>
       <c r="E18">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18">
-        <v>1.037378807936728</v>
+        <v>1.060391405444464</v>
       </c>
       <c r="G18">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H18">
-        <v>1.093463186024656</v>
+        <v>1.117099614120022</v>
       </c>
       <c r="I18">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J18">
-        <v>1.179373264997075</v>
+        <v>1.20632132508483</v>
       </c>
       <c r="K18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L18">
-        <v>1.648102362006173</v>
+        <v>1.23246330598014</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="N18">
-        <v>1.398453023321877</v>
+        <v>1.403554554982445</v>
       </c>
       <c r="O18">
+        <v>7</v>
+      </c>
+      <c r="P18">
+        <v>1.639880511277437</v>
+      </c>
+      <c r="Q18">
+        <v>4</v>
+      </c>
+      <c r="R18">
+        <v>1.514891059515569</v>
+      </c>
+      <c r="S18">
         <v>6</v>
       </c>
-      <c r="P18">
-        <v>1.697657751865507</v>
-      </c>
-      <c r="Q18">
-        <v>3</v>
-      </c>
-      <c r="R18">
-        <v>1.277551109076002</v>
-      </c>
-      <c r="S18">
-        <v>10</v>
-      </c>
       <c r="T18">
-        <v>1.393533678263558</v>
+        <v>1.342166896974554</v>
       </c>
       <c r="U18">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1681,64 +1681,64 @@
         <v>38</v>
       </c>
       <c r="B19">
-        <v>0.9519826680327619</v>
+        <v>0.9456353775836208</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19">
-        <v>0.9908333002734172</v>
+        <v>0.981404129205371</v>
       </c>
       <c r="E19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>1.046300645421349</v>
+        <v>1.031998194442571</v>
       </c>
       <c r="G19">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H19">
-        <v>1.130096880721081</v>
+        <v>1.106884943011991</v>
       </c>
       <c r="I19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J19">
-        <v>1.296677186617465</v>
+        <v>1.241651687131502</v>
       </c>
       <c r="K19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L19">
-        <v>1.583930773458039</v>
+        <v>1.315164588111806</v>
       </c>
       <c r="M19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N19">
-        <v>1.495960590255254</v>
+        <v>1.669706414282678</v>
       </c>
       <c r="O19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P19">
-        <v>1.809086325070371</v>
+        <v>2.034556140665266</v>
       </c>
       <c r="Q19">
         <v>2</v>
       </c>
       <c r="R19">
-        <v>1.489422113100455</v>
+        <v>1.930609029127617</v>
       </c>
       <c r="S19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T19">
-        <v>1.412136662791142</v>
+        <v>1.489586101449988</v>
       </c>
       <c r="U19">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1746,64 +1746,64 @@
         <v>39</v>
       </c>
       <c r="B20">
-        <v>0.9309183087267631</v>
+        <v>0.9167787971385479</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20">
-        <v>0.9539979300150869</v>
+        <v>0.9381688908442505</v>
       </c>
       <c r="E20">
+        <v>21</v>
+      </c>
+      <c r="F20">
+        <v>0.9714750530979754</v>
+      </c>
+      <c r="G20">
         <v>19</v>
       </c>
-      <c r="F20">
-        <v>0.9907221278810028</v>
-      </c>
-      <c r="G20">
-        <v>17</v>
-      </c>
       <c r="H20">
-        <v>1.049541281458969</v>
+        <v>1.023000313468716</v>
       </c>
       <c r="I20">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J20">
-        <v>1.170667817189366</v>
+        <v>1.116244226410379</v>
       </c>
       <c r="K20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L20">
-        <v>1.331757648017859</v>
+        <v>1.202690676693376</v>
       </c>
       <c r="M20">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="N20">
-        <v>1.42231290586699</v>
+        <v>1.455422677046836</v>
       </c>
       <c r="O20">
         <v>5</v>
       </c>
       <c r="P20">
-        <v>1.671795579490452</v>
+        <v>1.510560920130607</v>
       </c>
       <c r="Q20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R20">
-        <v>1.145150249417903</v>
+        <v>1.377228312518241</v>
       </c>
       <c r="S20">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="T20">
-        <v>0.9818393110882575</v>
+        <v>1.904138977574682</v>
       </c>
       <c r="U20">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1811,64 +1811,64 @@
         <v>40</v>
       </c>
       <c r="B21">
-        <v>0.8896688429754337</v>
+        <v>0.8862355777518247</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21">
-        <v>1.041343114631893</v>
+        <v>1.03410227275646</v>
       </c>
       <c r="E21">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F21">
-        <v>1.396447964959264</v>
+        <v>1.26436757425869</v>
       </c>
       <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>2.303028734642427</v>
+      </c>
+      <c r="I21">
         <v>1</v>
       </c>
-      <c r="H21">
-        <v>1.285007833386371</v>
-      </c>
-      <c r="I21">
-        <v>2</v>
-      </c>
       <c r="J21">
-        <v>1.027820191148586</v>
+        <v>1.051060472215689</v>
       </c>
       <c r="K21">
         <v>14</v>
       </c>
       <c r="L21">
-        <v>1.032189472924219</v>
+        <v>1.059303055579568</v>
       </c>
       <c r="M21">
         <v>14</v>
       </c>
       <c r="N21">
-        <v>1.036752099029469</v>
+        <v>1.06782567968914</v>
       </c>
       <c r="O21">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P21">
-        <v>1.041514892585601</v>
+        <v>1.07664264906357</v>
       </c>
       <c r="Q21">
         <v>14</v>
       </c>
       <c r="R21">
-        <v>1.04648520439176</v>
+        <v>1.085769344780236</v>
       </c>
       <c r="S21">
         <v>14</v>
       </c>
       <c r="T21">
-        <v>1.051670956863838</v>
+        <v>1.095222331247331</v>
       </c>
       <c r="U21">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -1876,64 +1876,64 @@
         <v>41</v>
       </c>
       <c r="B22">
-        <v>0.8766726158462499</v>
+        <v>0.868835145399964</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22">
-        <v>1.00620662890738</v>
+        <v>0.9060158342852838</v>
       </c>
       <c r="E22">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>0.957834209398276</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22">
+        <v>1.033641392212244</v>
+      </c>
+      <c r="I22">
         <v>14</v>
       </c>
-      <c r="F22">
-        <v>1.222503042147893</v>
-      </c>
-      <c r="G22">
+      <c r="J22">
+        <v>1.164684687445193</v>
+      </c>
+      <c r="K22">
+        <v>9</v>
+      </c>
+      <c r="L22">
+        <v>1.342364524181274</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>1.552898336158735</v>
+      </c>
+      <c r="O22">
+        <v>3</v>
+      </c>
+      <c r="P22">
+        <v>2.104261082074432</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1.705505910781421</v>
+      </c>
+      <c r="S22">
         <v>2</v>
       </c>
-      <c r="H22">
-        <v>1.628470627944004</v>
-      </c>
-      <c r="I22">
+      <c r="T22">
+        <v>2.165265548874677</v>
+      </c>
+      <c r="U22">
         <v>1</v>
-      </c>
-      <c r="J22">
-        <v>0.9765675359444477</v>
-      </c>
-      <c r="K22">
-        <v>18</v>
-      </c>
-      <c r="L22">
-        <v>0.9740372753529121</v>
-      </c>
-      <c r="M22">
-        <v>17</v>
-      </c>
-      <c r="N22">
-        <v>0.9716462184705723</v>
-      </c>
-      <c r="O22">
-        <v>17</v>
-      </c>
-      <c r="P22">
-        <v>0.9693919896063328</v>
-      </c>
-      <c r="Q22">
-        <v>17</v>
-      </c>
-      <c r="R22">
-        <v>0.9672724378244103</v>
-      </c>
-      <c r="S22">
-        <v>17</v>
-      </c>
-      <c r="T22">
-        <v>0.9652856289510503</v>
-      </c>
-      <c r="U22">
-        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1941,64 +1941,64 @@
         <v>42</v>
       </c>
       <c r="B23">
-        <v>0.8545961416134612</v>
+        <v>0.865634660056237</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23">
-        <v>0.8929669214547156</v>
+        <v>0.9868780641610638</v>
       </c>
       <c r="E23">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F23">
-        <v>0.9474592741523244</v>
+        <v>1.40990581073901</v>
       </c>
       <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1.434123396288106</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>0.955311977263289</v>
+      </c>
+      <c r="K23">
         <v>20</v>
       </c>
-      <c r="H23">
-        <v>1.029612492043481</v>
-      </c>
-      <c r="I23">
-        <v>15</v>
-      </c>
-      <c r="J23">
-        <v>1.189573019446696</v>
-      </c>
-      <c r="K23">
-        <v>7</v>
-      </c>
       <c r="L23">
-        <v>1.440820911903842</v>
+        <v>0.949592246083356</v>
       </c>
       <c r="M23">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="N23">
-        <v>1.473911859308604</v>
+        <v>0.944033906319945</v>
       </c>
       <c r="O23">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="P23">
-        <v>1.887447285068146</v>
+        <v>0.9386308766424152</v>
       </c>
       <c r="Q23">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R23">
-        <v>2.724349326285008</v>
+        <v>0.9333774098155753</v>
       </c>
       <c r="S23">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="T23">
-        <v>2.008859908325674</v>
+        <v>0.9282680697766033</v>
       </c>
       <c r="U23">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results after 10 executions
</commit_message>
<xml_diff>
--- a/outputs/paper/ARR_Rank.xlsx
+++ b/outputs/paper/ARR_Rank.xlsx
@@ -576,61 +576,61 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>1.096475584272148</v>
+        <v>1.096474665338817</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1.108945552742671</v>
+        <v>1.10894472136349</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1.129324259537674</v>
+        <v>1.129324404926565</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
       <c r="H2">
-        <v>1.160815804357349</v>
+        <v>1.1608180490128</v>
       </c>
       <c r="I2">
         <v>6</v>
       </c>
       <c r="J2">
-        <v>1.220392935599892</v>
+        <v>1.220403142791948</v>
       </c>
       <c r="K2">
         <v>5</v>
       </c>
       <c r="L2">
-        <v>1.207007661777844</v>
+        <v>1.207028826318944</v>
       </c>
       <c r="M2">
         <v>10</v>
       </c>
       <c r="N2">
-        <v>1.265981068401369</v>
+        <v>1.266016602577101</v>
       </c>
       <c r="O2">
         <v>10</v>
       </c>
       <c r="P2">
-        <v>1.364987252664707</v>
+        <v>1.365055893302424</v>
       </c>
       <c r="Q2">
         <v>9</v>
       </c>
       <c r="R2">
-        <v>1.375559274084418</v>
+        <v>1.37570871740984</v>
       </c>
       <c r="S2">
         <v>9</v>
       </c>
       <c r="T2">
-        <v>1.66287794110657</v>
+        <v>1.663417004985926</v>
       </c>
       <c r="U2">
         <v>4</v>
@@ -641,61 +641,61 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>1.083044553220067</v>
+        <v>1.083022255966642</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1.107323626900181</v>
+        <v>1.107275939820591</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
-        <v>1.140468958653252</v>
+        <v>1.140390702967093</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3">
-        <v>1.186884643582913</v>
+        <v>1.18676545590664</v>
       </c>
       <c r="I3">
         <v>3</v>
       </c>
       <c r="J3">
-        <v>1.272641677055092</v>
+        <v>1.27241514090511</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="L3">
-        <v>1.266604950497278</v>
+        <v>1.266391758919541</v>
       </c>
       <c r="M3">
         <v>6</v>
       </c>
       <c r="N3">
-        <v>1.353977844572786</v>
+        <v>1.353651210291811</v>
       </c>
       <c r="O3">
         <v>9</v>
       </c>
       <c r="P3">
-        <v>1.512181813345827</v>
+        <v>1.511503537084173</v>
       </c>
       <c r="Q3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R3">
-        <v>1.559643008779139</v>
+        <v>1.558912943509759</v>
       </c>
       <c r="S3">
         <v>4</v>
       </c>
       <c r="T3">
-        <v>1.795496870031311</v>
+        <v>1.791516357167215</v>
       </c>
       <c r="U3">
         <v>3</v>
@@ -706,61 +706,61 @@
         <v>23</v>
       </c>
       <c r="B4">
-        <v>1.061734415868065</v>
+        <v>1.061745573906169</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
-        <v>1.037835804742023</v>
+        <v>1.037857700612674</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4">
-        <v>1.018552709137146</v>
+        <v>1.018584979203556</v>
       </c>
       <c r="G4">
         <v>14</v>
       </c>
       <c r="H4">
-        <v>1.003177443884919</v>
+        <v>1.00321982689459</v>
       </c>
       <c r="I4">
         <v>16</v>
       </c>
       <c r="J4">
-        <v>0.991459677920928</v>
+        <v>0.991512062579606</v>
       </c>
       <c r="K4">
         <v>16</v>
       </c>
       <c r="L4">
-        <v>0.9835929892260958</v>
+        <v>0.983655488641324</v>
       </c>
       <c r="M4">
         <v>16</v>
       </c>
       <c r="N4">
-        <v>0.9805246370373211</v>
+        <v>0.9805977421925964</v>
       </c>
       <c r="O4">
         <v>16</v>
       </c>
       <c r="P4">
-        <v>0.9854805607832389</v>
+        <v>0.9855655710937999</v>
       </c>
       <c r="Q4">
         <v>15</v>
       </c>
       <c r="R4">
-        <v>1.0206703454613</v>
+        <v>1.020774193289638</v>
       </c>
       <c r="S4">
         <v>15</v>
       </c>
       <c r="T4">
-        <v>0.9323900882262983</v>
+        <v>0.9325217619890251</v>
       </c>
       <c r="U4">
         <v>19</v>
@@ -771,61 +771,61 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>1.06168206144241</v>
+        <v>1.061688788193455</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>1.037550890315733</v>
+        <v>1.037564199513352</v>
       </c>
       <c r="E5">
         <v>11</v>
       </c>
       <c r="F5">
-        <v>1.018067408332517</v>
+        <v>1.018087117860067</v>
       </c>
       <c r="G5">
         <v>15</v>
       </c>
       <c r="H5">
-        <v>1.002447521994901</v>
+        <v>1.002473451197556</v>
       </c>
       <c r="I5">
         <v>18</v>
       </c>
       <c r="J5">
-        <v>0.9903102060396979</v>
+        <v>0.9903421881301003</v>
       </c>
       <c r="K5">
         <v>17</v>
       </c>
       <c r="L5">
-        <v>0.9815798483004586</v>
+        <v>0.9816177248629291</v>
       </c>
       <c r="M5">
         <v>17</v>
       </c>
       <c r="N5">
-        <v>0.9765125137726514</v>
+        <v>0.9765560994020493</v>
       </c>
       <c r="O5">
         <v>17</v>
       </c>
       <c r="P5">
-        <v>0.975878102713619</v>
+        <v>0.9759270544665707</v>
       </c>
       <c r="Q5">
         <v>17</v>
       </c>
       <c r="R5">
-        <v>0.9815467970555257</v>
+        <v>0.9816000606888035</v>
       </c>
       <c r="S5">
         <v>17</v>
       </c>
       <c r="T5">
-        <v>0.9988408130274806</v>
+        <v>0.9988931316905049</v>
       </c>
       <c r="U5">
         <v>16</v>
@@ -836,61 +836,61 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>1.058952224396026</v>
+        <v>1.058946591094721</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>1.065463092552758</v>
+        <v>1.0654512645318</v>
       </c>
       <c r="E6">
         <v>7</v>
       </c>
       <c r="F6">
-        <v>1.077625891559313</v>
+        <v>1.077606923209818</v>
       </c>
       <c r="G6">
         <v>9</v>
       </c>
       <c r="H6">
-        <v>1.096365094036048</v>
+        <v>1.096337548500781</v>
       </c>
       <c r="I6">
         <v>12</v>
       </c>
       <c r="J6">
-        <v>1.125004877764473</v>
+        <v>1.124966747996333</v>
       </c>
       <c r="K6">
         <v>11</v>
       </c>
       <c r="L6">
-        <v>1.183237853029777</v>
+        <v>1.18319576151974</v>
       </c>
       <c r="M6">
         <v>12</v>
       </c>
       <c r="N6">
-        <v>1.150480176543564</v>
+        <v>1.15041105180571</v>
       </c>
       <c r="O6">
         <v>12</v>
       </c>
       <c r="P6">
-        <v>1.199207167687442</v>
+        <v>1.199064251574</v>
       </c>
       <c r="Q6">
         <v>12</v>
       </c>
       <c r="R6">
-        <v>1.335253020657419</v>
+        <v>1.333519827605152</v>
       </c>
       <c r="S6">
         <v>10</v>
       </c>
       <c r="T6">
-        <v>1.182581769876504</v>
+        <v>1.182525537537452</v>
       </c>
       <c r="U6">
         <v>12</v>
@@ -901,61 +901,61 @@
         <v>26</v>
       </c>
       <c r="B7">
-        <v>1.056713680158891</v>
+        <v>1.056704484520414</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7">
-        <v>1.034554507371336</v>
+        <v>1.034536625997518</v>
       </c>
       <c r="E7">
         <v>12</v>
       </c>
       <c r="F7">
-        <v>1.016927619901871</v>
+        <v>1.016901188656016</v>
       </c>
       <c r="G7">
         <v>16</v>
       </c>
       <c r="H7">
-        <v>1.003108048869777</v>
+        <v>1.003072894383181</v>
       </c>
       <c r="I7">
         <v>17</v>
       </c>
       <c r="J7">
-        <v>0.9927639577272055</v>
+        <v>0.9927195693118177</v>
       </c>
       <c r="K7">
         <v>15</v>
       </c>
       <c r="L7">
-        <v>0.985869993492374</v>
+        <v>0.9858153960562577</v>
       </c>
       <c r="M7">
         <v>15</v>
       </c>
       <c r="N7">
-        <v>0.9827444962927927</v>
+        <v>0.9826779456453772</v>
       </c>
       <c r="O7">
         <v>15</v>
       </c>
       <c r="P7">
-        <v>0.9842495027125165</v>
+        <v>0.9841677514543952</v>
       </c>
       <c r="Q7">
         <v>16</v>
       </c>
       <c r="R7">
-        <v>0.9924175904561233</v>
+        <v>0.9923138257728897</v>
       </c>
       <c r="S7">
         <v>16</v>
       </c>
       <c r="T7">
-        <v>1.012931142430802</v>
+        <v>1.012786960501726</v>
       </c>
       <c r="U7">
         <v>15</v>
@@ -966,61 +966,61 @@
         <v>27</v>
       </c>
       <c r="B8">
-        <v>1.054116764341472</v>
+        <v>1.054119152163282</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>1.049404659884196</v>
+        <v>1.049409425183663</v>
       </c>
       <c r="E8">
         <v>8</v>
       </c>
       <c r="F8">
-        <v>1.049724245589476</v>
+        <v>1.049731050558891</v>
       </c>
       <c r="G8">
         <v>12</v>
       </c>
       <c r="H8">
-        <v>1.05558859434869</v>
+        <v>1.055596636519758</v>
       </c>
       <c r="I8">
         <v>13</v>
       </c>
       <c r="J8">
-        <v>1.069426244902838</v>
+        <v>1.069433321948674</v>
       </c>
       <c r="K8">
         <v>13</v>
       </c>
       <c r="L8">
-        <v>1.105152946524391</v>
+        <v>1.105142901166795</v>
       </c>
       <c r="M8">
         <v>13</v>
       </c>
       <c r="N8">
-        <v>1.059667314329371</v>
+        <v>1.059690497643181</v>
       </c>
       <c r="O8">
         <v>14</v>
       </c>
       <c r="P8">
-        <v>1.077039746571793</v>
+        <v>1.077065376994016</v>
       </c>
       <c r="Q8">
         <v>13</v>
       </c>
       <c r="R8">
-        <v>1.103058796180808</v>
+        <v>1.103086263561399</v>
       </c>
       <c r="S8">
         <v>13</v>
       </c>
       <c r="T8">
-        <v>1.143367150280038</v>
+        <v>1.143395218196588</v>
       </c>
       <c r="U8">
         <v>13</v>
@@ -1031,61 +1031,61 @@
         <v>28</v>
       </c>
       <c r="B9">
-        <v>1.050726750301721</v>
+        <v>1.050722538850065</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9">
-        <v>1.070241863579622</v>
+        <v>1.070233507891533</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
       <c r="F9">
-        <v>1.096334869188334</v>
+        <v>1.096321892899109</v>
       </c>
       <c r="G9">
         <v>8</v>
       </c>
       <c r="H9">
-        <v>1.130784761306789</v>
+        <v>1.130765748644752</v>
       </c>
       <c r="I9">
         <v>8</v>
       </c>
       <c r="J9">
-        <v>1.178609731005983</v>
+        <v>1.178580289948267</v>
       </c>
       <c r="K9">
         <v>8</v>
       </c>
       <c r="L9">
-        <v>1.270138820504554</v>
+        <v>1.270050665192612</v>
       </c>
       <c r="M9">
         <v>5</v>
       </c>
       <c r="N9">
-        <v>1.24367355569919</v>
+        <v>1.243648323579658</v>
       </c>
       <c r="O9">
         <v>11</v>
       </c>
       <c r="P9">
-        <v>1.346383320853301</v>
+        <v>1.346338694472193</v>
       </c>
       <c r="Q9">
         <v>11</v>
       </c>
       <c r="R9">
-        <v>1.273831233825431</v>
+        <v>1.273805744280726</v>
       </c>
       <c r="S9">
         <v>11</v>
       </c>
       <c r="T9">
-        <v>1.409481862005331</v>
+        <v>1.409453092650331</v>
       </c>
       <c r="U9">
         <v>7</v>
@@ -1096,61 +1096,61 @@
         <v>29</v>
       </c>
       <c r="B10">
-        <v>1.048957970551326</v>
+        <v>1.048951478623134</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10">
-        <v>1.075237682281905</v>
+        <v>1.075226021948847</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10">
-        <v>1.111411994790438</v>
+        <v>1.111397200029665</v>
       </c>
       <c r="G10">
         <v>6</v>
       </c>
       <c r="H10">
-        <v>1.162695164216764</v>
+        <v>1.162681434032632</v>
       </c>
       <c r="I10">
         <v>5</v>
       </c>
       <c r="J10">
-        <v>1.245891759042389</v>
+        <v>1.245894650572193</v>
       </c>
       <c r="K10">
         <v>3</v>
       </c>
       <c r="L10">
-        <v>1.264148389521569</v>
+        <v>1.264167712853274</v>
       </c>
       <c r="M10">
         <v>7</v>
       </c>
       <c r="N10">
-        <v>1.430020511418638</v>
+        <v>1.430059419879125</v>
       </c>
       <c r="O10">
         <v>6</v>
       </c>
       <c r="P10">
-        <v>1.680539705797795</v>
+        <v>1.68135039247702</v>
       </c>
       <c r="Q10">
         <v>3</v>
       </c>
       <c r="R10">
-        <v>1.261204666133432</v>
+        <v>1.261298205416699</v>
       </c>
       <c r="S10">
         <v>12</v>
       </c>
       <c r="T10">
-        <v>1.358376595201438</v>
+        <v>1.35958657195625</v>
       </c>
       <c r="U10">
         <v>8</v>
@@ -1161,61 +1161,61 @@
         <v>30</v>
       </c>
       <c r="B11">
-        <v>1.047267780464769</v>
+        <v>1.047254188672275</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>1.069473909618415</v>
+        <v>1.069445680963792</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
       <c r="F11">
-        <v>1.100216769371</v>
+        <v>1.100171807377622</v>
       </c>
       <c r="G11">
         <v>7</v>
       </c>
       <c r="H11">
-        <v>1.143319471052173</v>
+        <v>1.143253564552536</v>
       </c>
       <c r="I11">
         <v>7</v>
       </c>
       <c r="J11">
-        <v>1.209856898043752</v>
+        <v>1.209758496094248</v>
       </c>
       <c r="K11">
         <v>6</v>
       </c>
       <c r="L11">
-        <v>1.394088693868389</v>
+        <v>1.393788920152632</v>
       </c>
       <c r="M11">
         <v>2</v>
       </c>
       <c r="N11">
-        <v>1.375323296151508</v>
+        <v>1.375199591811777</v>
       </c>
       <c r="O11">
         <v>8</v>
       </c>
       <c r="P11">
-        <v>1.468298542163537</v>
+        <v>1.468082121219824</v>
       </c>
       <c r="Q11">
         <v>8</v>
       </c>
       <c r="R11">
-        <v>1.68355630308076</v>
+        <v>1.682990190695235</v>
       </c>
       <c r="S11">
         <v>3</v>
       </c>
       <c r="T11">
-        <v>1.237751447238716</v>
+        <v>1.237559667936847</v>
       </c>
       <c r="U11">
         <v>11</v>
@@ -1226,61 +1226,61 @@
         <v>31</v>
       </c>
       <c r="B12">
-        <v>1.031457901664917</v>
+        <v>1.03144341906115</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12">
-        <v>1.067224637040966</v>
+        <v>1.067193501368029</v>
       </c>
       <c r="E12">
         <v>6</v>
       </c>
       <c r="F12">
-        <v>1.115029292175002</v>
+        <v>1.114977175449969</v>
       </c>
       <c r="G12">
         <v>5</v>
       </c>
       <c r="H12">
-        <v>1.182629051574606</v>
+        <v>1.182545978152282</v>
       </c>
       <c r="I12">
         <v>4</v>
       </c>
       <c r="J12">
-        <v>1.300514992012559</v>
+        <v>1.300352620391178</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12">
-        <v>1.529602474709112</v>
+        <v>1.529759798535003</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
       <c r="N12">
-        <v>1.581367019433214</v>
+        <v>1.580978530259384</v>
       </c>
       <c r="O12">
         <v>2</v>
       </c>
       <c r="P12">
-        <v>1.490724495672699</v>
+        <v>1.489380891301815</v>
       </c>
       <c r="Q12">
         <v>7</v>
       </c>
       <c r="R12">
-        <v>1.548093417153733</v>
+        <v>1.542184972098407</v>
       </c>
       <c r="S12">
         <v>5</v>
       </c>
       <c r="T12">
-        <v>1.292809807928736</v>
+        <v>1.292561178217637</v>
       </c>
       <c r="U12">
         <v>10</v>
@@ -1291,61 +1291,61 @@
         <v>32</v>
       </c>
       <c r="B13">
-        <v>1.02803013132057</v>
+        <v>1.028036504987708</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13">
-        <v>1.004406533409582</v>
+        <v>1.004419191837083</v>
       </c>
       <c r="E13">
         <v>15</v>
       </c>
       <c r="F13">
-        <v>0.9853487253403637</v>
+        <v>0.9853675100072259</v>
       </c>
       <c r="G13">
         <v>17</v>
       </c>
       <c r="H13">
-        <v>0.9700741443075002</v>
+        <v>0.9700988901995993</v>
       </c>
       <c r="I13">
         <v>19</v>
       </c>
       <c r="J13">
-        <v>0.958192738465202</v>
+        <v>0.9582233283200213</v>
       </c>
       <c r="K13">
         <v>18</v>
       </c>
       <c r="L13">
-        <v>0.9496066281806315</v>
+        <v>0.9496430658159992</v>
       </c>
       <c r="M13">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N13">
-        <v>0.9445245112836312</v>
+        <v>0.9445670669874756</v>
       </c>
       <c r="O13">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P13">
-        <v>0.9436067279322886</v>
+        <v>0.9436563018845101</v>
       </c>
       <c r="Q13">
         <v>19</v>
       </c>
       <c r="R13">
-        <v>0.9484096399780769</v>
+        <v>0.948468876476159</v>
       </c>
       <c r="S13">
         <v>19</v>
       </c>
       <c r="T13">
-        <v>0.9628940909179671</v>
+        <v>0.9629719424982068</v>
       </c>
       <c r="U13">
         <v>18</v>
@@ -1356,61 +1356,61 @@
         <v>33</v>
       </c>
       <c r="B14">
-        <v>1.025397174108525</v>
+        <v>1.025391088581729</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14">
-        <v>1.043941349256491</v>
+        <v>1.043928862412607</v>
       </c>
       <c r="E14">
         <v>9</v>
       </c>
       <c r="F14">
-        <v>1.069478536171666</v>
+        <v>1.069458866922968</v>
       </c>
       <c r="G14">
         <v>10</v>
       </c>
       <c r="H14">
-        <v>1.104251319208093</v>
+        <v>1.104222937124544</v>
       </c>
       <c r="I14">
         <v>11</v>
       </c>
       <c r="J14">
-        <v>1.153821434507214</v>
+        <v>1.153781014898929</v>
       </c>
       <c r="K14">
         <v>10</v>
       </c>
       <c r="L14">
-        <v>1.238993940173276</v>
+        <v>1.238929727178076</v>
       </c>
       <c r="M14">
         <v>8</v>
       </c>
       <c r="N14">
-        <v>1.479604300668834</v>
+        <v>1.479615622191293</v>
       </c>
       <c r="O14">
         <v>4</v>
       </c>
       <c r="P14">
-        <v>1.364321213831999</v>
+        <v>1.364221910709791</v>
       </c>
       <c r="Q14">
         <v>10</v>
       </c>
       <c r="R14">
-        <v>1.497051654402041</v>
+        <v>1.496723922700098</v>
       </c>
       <c r="S14">
         <v>7</v>
       </c>
       <c r="T14">
-        <v>1.539732463524918</v>
+        <v>1.539948885689952</v>
       </c>
       <c r="U14">
         <v>5</v>
@@ -1421,61 +1421,61 @@
         <v>34</v>
       </c>
       <c r="B15">
-        <v>1.020342092729119</v>
+        <v>1.020339713264287</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15">
-        <v>0.9983176340959177</v>
+        <v>0.998313179918178</v>
       </c>
       <c r="E15">
         <v>16</v>
       </c>
       <c r="F15">
-        <v>0.9808941152373433</v>
+        <v>0.9808877030727721</v>
       </c>
       <c r="G15">
         <v>18</v>
       </c>
       <c r="H15">
-        <v>0.9673176043190614</v>
+        <v>0.9673092147433143</v>
       </c>
       <c r="I15">
         <v>20</v>
       </c>
       <c r="J15">
-        <v>0.9572339481996606</v>
+        <v>0.9572234192780398</v>
       </c>
       <c r="K15">
         <v>19</v>
       </c>
       <c r="L15">
-        <v>0.9505937258283339</v>
+        <v>0.9505806919004194</v>
       </c>
       <c r="M15">
         <v>18</v>
       </c>
       <c r="N15">
-        <v>0.9476782309786268</v>
+        <v>0.9476619641222678</v>
       </c>
       <c r="O15">
         <v>18</v>
       </c>
       <c r="P15">
-        <v>0.9492689631842507</v>
+        <v>0.9492479707121934</v>
       </c>
       <c r="Q15">
         <v>18</v>
       </c>
       <c r="R15">
-        <v>0.9571481565715342</v>
+        <v>0.9571189989018565</v>
       </c>
       <c r="S15">
         <v>18</v>
       </c>
       <c r="T15">
-        <v>0.975744149709886</v>
+        <v>0.9756968754582487</v>
       </c>
       <c r="U15">
         <v>17</v>
@@ -1486,61 +1486,61 @@
         <v>35</v>
       </c>
       <c r="B16">
-        <v>1.008154569172945</v>
+        <v>1.008155115257226</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16">
-        <v>0.9485495844941579</v>
+        <v>0.9485505117634946</v>
       </c>
       <c r="E16">
         <v>19</v>
       </c>
       <c r="F16">
-        <v>0.8977653274531157</v>
+        <v>0.8977664175234169</v>
       </c>
       <c r="G16">
         <v>22</v>
       </c>
       <c r="H16">
-        <v>0.853849693151205</v>
+        <v>0.8538507333884928</v>
       </c>
       <c r="I16">
         <v>22</v>
       </c>
       <c r="J16">
-        <v>0.8154890626851603</v>
+        <v>0.8154898544014137</v>
       </c>
       <c r="K16">
         <v>22</v>
       </c>
       <c r="L16">
-        <v>0.7817637863505321</v>
+        <v>0.7817641362013144</v>
       </c>
       <c r="M16">
         <v>22</v>
       </c>
       <c r="N16">
-        <v>0.7520267449376651</v>
+        <v>0.7520264480293543</v>
       </c>
       <c r="O16">
         <v>22</v>
       </c>
       <c r="P16">
-        <v>0.7258457981421534</v>
+        <v>0.7258446114260571</v>
       </c>
       <c r="Q16">
         <v>22</v>
       </c>
       <c r="R16">
-        <v>0.7029950149234478</v>
+        <v>0.7029926105521236</v>
       </c>
       <c r="S16">
         <v>22</v>
       </c>
       <c r="T16">
-        <v>0.6835138664776848</v>
+        <v>0.6835097337383212</v>
       </c>
       <c r="U16">
         <v>22</v>
@@ -1551,61 +1551,61 @@
         <v>36</v>
       </c>
       <c r="B17">
-        <v>0.9991030613116985</v>
+        <v>0.9991207907474821</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17">
-        <v>0.9443835163561156</v>
+        <v>0.9444168994696811</v>
       </c>
       <c r="E17">
         <v>20</v>
       </c>
       <c r="F17">
-        <v>0.8988049366539033</v>
+        <v>0.8988524598005077</v>
       </c>
       <c r="G17">
         <v>21</v>
       </c>
       <c r="H17">
-        <v>0.8600908741308049</v>
+        <v>0.860151455113592</v>
       </c>
       <c r="I17">
         <v>21</v>
       </c>
       <c r="J17">
-        <v>0.8267890765996453</v>
+        <v>0.8268620074129732</v>
       </c>
       <c r="K17">
         <v>21</v>
       </c>
       <c r="L17">
-        <v>0.7979339627052328</v>
+        <v>0.7980189154137323</v>
       </c>
       <c r="M17">
         <v>21</v>
       </c>
       <c r="N17">
-        <v>0.7728888306607634</v>
+        <v>0.7729859474387343</v>
       </c>
       <c r="O17">
         <v>21</v>
       </c>
       <c r="P17">
-        <v>0.7512814850583902</v>
+        <v>0.7513916303641276</v>
       </c>
       <c r="Q17">
         <v>21</v>
       </c>
       <c r="R17">
-        <v>0.7330205308753661</v>
+        <v>0.7331459538298704</v>
       </c>
       <c r="S17">
         <v>21</v>
       </c>
       <c r="T17">
-        <v>0.7184594622480753</v>
+        <v>0.7186058030645526</v>
       </c>
       <c r="U17">
         <v>21</v>
@@ -1616,61 +1616,61 @@
         <v>37</v>
       </c>
       <c r="B18">
-        <v>0.9881495817969133</v>
+        <v>0.9881547420529664</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18">
-        <v>1.019202571983889</v>
+        <v>1.019213128869054</v>
       </c>
       <c r="E18">
         <v>14</v>
       </c>
       <c r="F18">
-        <v>1.060391405444464</v>
+        <v>1.060407425170527</v>
       </c>
       <c r="G18">
         <v>11</v>
       </c>
       <c r="H18">
-        <v>1.117099614120022</v>
+        <v>1.117120568926281</v>
       </c>
       <c r="I18">
         <v>9</v>
       </c>
       <c r="J18">
-        <v>1.20632132508483</v>
+        <v>1.206342911885919</v>
       </c>
       <c r="K18">
         <v>7</v>
       </c>
       <c r="L18">
-        <v>1.23246330598014</v>
+        <v>1.232504125734102</v>
       </c>
       <c r="M18">
         <v>9</v>
       </c>
       <c r="N18">
-        <v>1.403554554982445</v>
+        <v>1.40359016982021</v>
       </c>
       <c r="O18">
         <v>7</v>
       </c>
       <c r="P18">
-        <v>1.639880511277437</v>
+        <v>1.639800751853556</v>
       </c>
       <c r="Q18">
         <v>4</v>
       </c>
       <c r="R18">
-        <v>1.514891059515569</v>
+        <v>1.513464902528668</v>
       </c>
       <c r="S18">
         <v>6</v>
       </c>
       <c r="T18">
-        <v>1.342166896974554</v>
+        <v>1.342163052973084</v>
       </c>
       <c r="U18">
         <v>9</v>
@@ -1681,61 +1681,61 @@
         <v>38</v>
       </c>
       <c r="B19">
-        <v>0.9456353775836208</v>
+        <v>0.9456382359013619</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19">
-        <v>0.981404129205371</v>
+        <v>0.9814145162479652</v>
       </c>
       <c r="E19">
         <v>18</v>
       </c>
       <c r="F19">
-        <v>1.031998194442571</v>
+        <v>1.032024828871365</v>
       </c>
       <c r="G19">
         <v>13</v>
       </c>
       <c r="H19">
-        <v>1.106884943011991</v>
+        <v>1.106948630190063</v>
       </c>
       <c r="I19">
         <v>10</v>
       </c>
       <c r="J19">
-        <v>1.241651687131502</v>
+        <v>1.241868448171446</v>
       </c>
       <c r="K19">
         <v>4</v>
       </c>
       <c r="L19">
-        <v>1.315164588111806</v>
+        <v>1.315625887856902</v>
       </c>
       <c r="M19">
         <v>4</v>
       </c>
       <c r="N19">
-        <v>1.669706414282678</v>
+        <v>1.672853753204487</v>
       </c>
       <c r="O19">
         <v>1</v>
       </c>
       <c r="P19">
-        <v>2.034556140665266</v>
+        <v>2.04116327583166</v>
       </c>
       <c r="Q19">
         <v>2</v>
       </c>
       <c r="R19">
-        <v>1.930609029127617</v>
+        <v>1.934404999236109</v>
       </c>
       <c r="S19">
         <v>1</v>
       </c>
       <c r="T19">
-        <v>1.489586101449988</v>
+        <v>1.490034693751237</v>
       </c>
       <c r="U19">
         <v>6</v>
@@ -1746,61 +1746,61 @@
         <v>39</v>
       </c>
       <c r="B20">
-        <v>0.9167787971385479</v>
+        <v>0.9167715080479785</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20">
-        <v>0.9381688908442505</v>
+        <v>0.9381552067488531</v>
       </c>
       <c r="E20">
         <v>21</v>
       </c>
       <c r="F20">
-        <v>0.9714750530979754</v>
+        <v>0.9714566616074976</v>
       </c>
       <c r="G20">
         <v>19</v>
       </c>
       <c r="H20">
-        <v>1.023000313468716</v>
+        <v>1.022982135805227</v>
       </c>
       <c r="I20">
         <v>15</v>
       </c>
       <c r="J20">
-        <v>1.116244226410379</v>
+        <v>1.116260401711465</v>
       </c>
       <c r="K20">
         <v>12</v>
       </c>
       <c r="L20">
-        <v>1.202690676693376</v>
+        <v>1.202758893360648</v>
       </c>
       <c r="M20">
         <v>11</v>
       </c>
       <c r="N20">
-        <v>1.455422677046836</v>
+        <v>1.455938067114457</v>
       </c>
       <c r="O20">
         <v>5</v>
       </c>
       <c r="P20">
-        <v>1.510560920130607</v>
+        <v>1.511558134447908</v>
       </c>
       <c r="Q20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R20">
-        <v>1.377228312518241</v>
+        <v>1.377021504078443</v>
       </c>
       <c r="S20">
         <v>8</v>
       </c>
       <c r="T20">
-        <v>1.904138977574682</v>
+        <v>1.907044442224902</v>
       </c>
       <c r="U20">
         <v>2</v>
@@ -1811,61 +1811,61 @@
         <v>40</v>
       </c>
       <c r="B21">
-        <v>0.8862355777518247</v>
+        <v>0.8861818479335888</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21">
-        <v>1.03410227275646</v>
+        <v>1.033840563821772</v>
       </c>
       <c r="E21">
         <v>13</v>
       </c>
       <c r="F21">
-        <v>1.26436757425869</v>
+        <v>1.262497690425466</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="H21">
-        <v>2.303028734642427</v>
+        <v>2.112776961373534</v>
       </c>
       <c r="I21">
         <v>1</v>
       </c>
       <c r="J21">
-        <v>1.051060472215689</v>
+        <v>1.050510565625022</v>
       </c>
       <c r="K21">
         <v>14</v>
       </c>
       <c r="L21">
-        <v>1.059303055579568</v>
+        <v>1.058624765588463</v>
       </c>
       <c r="M21">
         <v>14</v>
       </c>
       <c r="N21">
-        <v>1.06782567968914</v>
+        <v>1.067011727084508</v>
       </c>
       <c r="O21">
         <v>13</v>
       </c>
       <c r="P21">
-        <v>1.07664264906357</v>
+        <v>1.075685163447281</v>
       </c>
       <c r="Q21">
         <v>14</v>
       </c>
       <c r="R21">
-        <v>1.085769344780236</v>
+        <v>1.084659802909362</v>
       </c>
       <c r="S21">
         <v>14</v>
       </c>
       <c r="T21">
-        <v>1.095222331247331</v>
+        <v>1.093951487382074</v>
       </c>
       <c r="U21">
         <v>14</v>
@@ -1876,61 +1876,61 @@
         <v>41</v>
       </c>
       <c r="B22">
-        <v>0.868835145399964</v>
+        <v>0.8688503425418287</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22">
-        <v>0.9060158342852838</v>
+        <v>0.9060496013461611</v>
       </c>
       <c r="E22">
         <v>22</v>
       </c>
       <c r="F22">
-        <v>0.957834209398276</v>
+        <v>0.9578930201365695</v>
       </c>
       <c r="G22">
         <v>20</v>
       </c>
       <c r="H22">
-        <v>1.033641392212244</v>
+        <v>1.033739709947586</v>
       </c>
       <c r="I22">
         <v>14</v>
       </c>
       <c r="J22">
-        <v>1.164684687445193</v>
+        <v>1.164884747189969</v>
       </c>
       <c r="K22">
         <v>9</v>
       </c>
       <c r="L22">
-        <v>1.342364524181274</v>
+        <v>1.342783007585531</v>
       </c>
       <c r="M22">
         <v>3</v>
       </c>
       <c r="N22">
-        <v>1.552898336158735</v>
+        <v>1.55394031054286</v>
       </c>
       <c r="O22">
         <v>3</v>
       </c>
       <c r="P22">
-        <v>2.104261082074432</v>
+        <v>2.105979474109558</v>
       </c>
       <c r="Q22">
         <v>1</v>
       </c>
       <c r="R22">
-        <v>1.705505910781421</v>
+        <v>1.705390927280749</v>
       </c>
       <c r="S22">
         <v>2</v>
       </c>
       <c r="T22">
-        <v>2.165265548874677</v>
+        <v>2.163442848023826</v>
       </c>
       <c r="U22">
         <v>1</v>
@@ -1941,61 +1941,61 @@
         <v>42</v>
       </c>
       <c r="B23">
-        <v>0.865634660056237</v>
+        <v>0.8657029543646813</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23">
-        <v>0.9868780641610638</v>
+        <v>0.987156304598361</v>
       </c>
       <c r="E23">
         <v>17</v>
       </c>
       <c r="F23">
-        <v>1.40990581073901</v>
+        <v>1.431552262678988</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23">
-        <v>1.434123396288106</v>
+        <v>1.438431800693735</v>
       </c>
       <c r="I23">
         <v>2</v>
       </c>
       <c r="J23">
-        <v>0.955311977263289</v>
+        <v>0.9557315924401212</v>
       </c>
       <c r="K23">
         <v>20</v>
       </c>
       <c r="L23">
-        <v>0.949592246083356</v>
+        <v>0.9500850218797894</v>
       </c>
       <c r="M23">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N23">
-        <v>0.944033906319945</v>
+        <v>0.9445967659506198</v>
       </c>
       <c r="O23">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P23">
-        <v>0.9386308766424152</v>
+        <v>0.9392609295069081</v>
       </c>
       <c r="Q23">
         <v>20</v>
       </c>
       <c r="R23">
-        <v>0.9333774098155753</v>
+        <v>0.9340719377800549</v>
       </c>
       <c r="S23">
         <v>20</v>
       </c>
       <c r="T23">
-        <v>0.9282680697766033</v>
+        <v>0.929024514661394</v>
       </c>
       <c r="U23">
         <v>20</v>

</xml_diff>